<commit_message>
Update v5.1.29 - Scripts de deploy automático y mejoras UI
</commit_message>
<xml_diff>
--- a/TABLA DE ACTIVACIONES (005).xlsx
+++ b/TABLA DE ACTIVACIONES (005).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documentos\Programas\VentasProui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07D093A7-CE1A-4594-96A0-5F49C23E21B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC30483-0BF6-4044-808D-B952E7D743D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t>MESES</t>
   </si>
   <si>
-    <t>SS SOLUTIONS</t>
-  </si>
-  <si>
     <t>CRP1</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t xml:space="preserve">OSVALDO RIVERA Y ASOCIADOS </t>
   </si>
   <si>
-    <t>135</t>
-  </si>
-  <si>
     <t>787-204-1494</t>
   </si>
   <si>
@@ -178,6 +172,12 @@
   </si>
   <si>
     <t>CREDITO DE $1000</t>
+  </si>
+  <si>
+    <t>DAYANA</t>
+  </si>
+  <si>
+    <t>43.33</t>
   </si>
 </sst>
 </file>
@@ -635,13 +635,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>587647</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>327932</xdr:rowOff>
@@ -976,37 +976,36 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P16"/>
+  <dimension ref="B1:Q16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="21" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
-    <col min="4" max="4" width="69.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="23" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19" style="24" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="21.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" customWidth="1"/>
-    <col min="16" max="16" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" style="21" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="5" max="5" width="69.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="23" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19" style="24" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="2:17" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
       <c r="C1" s="33"/>
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
@@ -1021,315 +1020,315 @@
       <c r="N1" s="33"/>
       <c r="O1" s="33"/>
       <c r="P1" s="33"/>
-    </row>
-    <row r="3" spans="1:16" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="28" t="s">
+      <c r="Q1" s="33"/>
+    </row>
+    <row r="3" spans="2:17" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B3" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="30"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29" t="s">
+        <v>47</v>
+      </c>
       <c r="E3" s="30"/>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="30"/>
+      <c r="K3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="34" t="s">
+      <c r="L3" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="34"/>
-    </row>
-    <row r="4" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="28" t="s">
+      <c r="M3" s="34"/>
+    </row>
+    <row r="4" spans="2:17" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="31">
+      <c r="C4" s="28"/>
+      <c r="D4" s="31">
         <v>60043</v>
       </c>
-      <c r="D4" s="32"/>
       <c r="E4" s="32"/>
       <c r="F4" s="32"/>
       <c r="G4" s="32"/>
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:16" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="28" t="s">
+      <c r="J4" s="32"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="2:17" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="36">
+      <c r="C5" s="28"/>
+      <c r="D5" s="36">
         <v>705088973</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="3"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="28" t="s">
+      <c r="J5" s="3"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="2:17" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="28" t="s">
+      <c r="J6" s="2"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="2:17" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="2"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="35"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8"/>
-      <c r="F8"/>
-      <c r="H8"/>
-      <c r="I8" s="6"/>
+      <c r="C8"/>
+      <c r="G8"/>
+      <c r="I8"/>
       <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9"/>
-      <c r="F9"/>
-      <c r="H9"/>
-      <c r="J9"/>
-    </row>
-    <row r="10" spans="1:16" s="13" customFormat="1" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="C9"/>
+      <c r="G9"/>
+      <c r="I9"/>
+      <c r="K9"/>
+    </row>
+    <row r="10" spans="2:17" s="13" customFormat="1" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="F10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="I10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="J10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="K10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="L10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="M10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="N10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="O10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="P10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="P10" s="12" t="s">
+      <c r="Q10" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="18" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="2:17" s="18" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="D11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q11" s="27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" s="18" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C12" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="F12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="O12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="P12" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q12" s="27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" s="18" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="C13" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="K13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="O13" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q13" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="M11" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="N11" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="O11" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="P11" s="27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="18" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="M12" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="O12" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="P12" s="27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" s="18" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="L13" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="M13" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="N13" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="O13" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13" s="27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" s="18" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="25"/>
-      <c r="B14" s="26"/>
+    </row>
+    <row r="14" spans="2:17" s="18" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="25"/>
       <c r="C14" s="26"/>
-      <c r="D14" s="15"/>
+      <c r="D14" s="26"/>
       <c r="E14" s="15"/>
-      <c r="F14" s="16"/>
+      <c r="F14" s="15"/>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
@@ -1337,17 +1336,17 @@
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="27"/>
-    </row>
-    <row r="15" spans="1:16" s="18" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="27"/>
+    </row>
+    <row r="15" spans="2:17" s="18" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="25"/>
       <c r="C15" s="26"/>
-      <c r="D15" s="15"/>
+      <c r="D15" s="26"/>
       <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
@@ -1355,17 +1354,17 @@
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="27"/>
-    </row>
-    <row r="16" spans="1:16" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="27"/>
+    </row>
+    <row r="16" spans="2:17" s="18" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="19"/>
       <c r="C16" s="20"/>
-      <c r="D16" s="15"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
+      <c r="F16" s="15"/>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
       <c r="I16" s="16"/>
@@ -1373,27 +1372,28 @@
       <c r="K16" s="16"/>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="15"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D3:J3"/>
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="31" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="29" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>